<commit_message>
add score of Li Meng Yong
</commit_message>
<xml_diff>
--- a/quize/scores/scores.xlsx
+++ b/quize/scores/scores.xlsx
@@ -565,8 +565,8 @@
   <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2175,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>9</v>
@@ -2184,31 +2184,31 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="V24">
         <f>SUM(C24:U24)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25">
         <v>9</v>
@@ -2313,7 +2313,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C26">
         <v>9</v>
@@ -2382,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C27">
         <v>9</v>
@@ -2412,10 +2412,10 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -2443,12 +2443,15 @@
       </c>
       <c r="V27">
         <f>SUM(C27:U27)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>9</v>
@@ -2513,20 +2516,77 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
         <v>0</v>
       </c>
       <c r="V29">
         <f>SUM(C29:U29)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2538,7 +2598,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2550,7 +2610,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -2562,7 +2622,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2574,7 +2634,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2621,9 +2681,6 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
       <c r="B38" t="s">
         <v>43</v>
       </c>
@@ -2650,7 +2707,7 @@
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>SUM(A2:A39)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B40">
         <f>COUNTA(B2:B39)</f>
@@ -2677,7 +2734,7 @@
       </c>
       <c r="V41">
         <f>COUNTIFS(V2:V39,"&gt;16",V2:V39,"&lt;=26")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
@@ -2695,7 +2752,7 @@
       <sortCondition descending="1" ref="V1:V39"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:V39">
+  <sortState ref="B2:V39">
     <sortCondition descending="1" ref="V2:V39"/>
     <sortCondition ref="B2:B39"/>
   </sortState>

</xml_diff>